<commit_message>
Google Address search query solve
</commit_message>
<xml_diff>
--- a/src/main/resources/excelfiles/VerifyCustomers.xlsx
+++ b/src/main/resources/excelfiles/VerifyCustomers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7740" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>TestCases</t>
   </si>
@@ -63,6 +63,12 @@
     <t>Leave all fields blank and check the validation messages</t>
   </si>
   <si>
+    <t>Sharad Pawar</t>
+  </si>
+  <si>
+    <t>sharad@yopmail.com</t>
+  </si>
+  <si>
     <t>Jamnagar, Gujarat, India</t>
   </si>
   <si>
@@ -81,7 +87,13 @@
     <t>4852 Spring St</t>
   </si>
   <si>
-    <t>Jamnagar</t>
+    <t>Verify Do Later button</t>
+  </si>
+  <si>
+    <t>Lillian Ward</t>
+  </si>
+  <si>
+    <t>ward@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -89,10 +101,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -119,6 +131,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -135,40 +155,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -197,21 +186,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -226,6 +200,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -234,6 +223,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -241,15 +245,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,25 +282,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,60 +444,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -366,85 +456,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,6 +467,54 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -499,54 +559,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -558,148 +570,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1094,7 +1106,7 @@
   <sheetPr/>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -1138,11 +1150,23 @@
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1">
+        <v>7456965485</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="sharad@yopmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1151,13 +1175,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.2857142857143" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="32.2857142857143" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="32.2857142857143" style="2" customWidth="1"/>
     <col min="2" max="2" width="58.1428571428571" style="2" customWidth="1"/>
@@ -1195,30 +1219,57 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1">
         <v>1590264569</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7412589512</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="lloyd@yopmail.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="ward@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>